<commit_message>
multiple browser code added
</commit_message>
<xml_diff>
--- a/DataSheet/Mars.xlsx
+++ b/DataSheet/Mars.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyotimadan/Documents/Projects/CSharpProject/Mars/DataSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EEE7A2-7CFB-6349-B5F7-E00027488965}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452DBA3E-A3F8-9441-B2A5-1C83041BBC35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="3" xr2:uid="{DF65A25B-7158-E041-B64A-E7FDC7345767}"/>
+    <workbookView xWindow="300" yWindow="540" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{DF65A25B-7158-E041-B64A-E7FDC7345767}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="ShareSkillTestData" sheetId="2" r:id="rId2"/>
-    <sheet name="ManageListingsTestData" sheetId="3" r:id="rId3"/>
-    <sheet name="ManageRequestsTestData" sheetId="9" r:id="rId4"/>
-    <sheet name="ProfileTestData" sheetId="4" r:id="rId5"/>
-    <sheet name="SearchTestData" sheetId="5" r:id="rId6"/>
-    <sheet name="ChatTestData" sheetId="6" r:id="rId7"/>
-    <sheet name="ServiceDetailTestData" sheetId="7" r:id="rId8"/>
-    <sheet name="NotificationTestData" sheetId="8" r:id="rId9"/>
+    <sheet name="ChangePasswordTestData" sheetId="10" r:id="rId2"/>
+    <sheet name="ShareSkillTestData" sheetId="2" r:id="rId3"/>
+    <sheet name="ManageListingsTestData" sheetId="3" r:id="rId4"/>
+    <sheet name="ManageRequestsTestData" sheetId="9" r:id="rId5"/>
+    <sheet name="ProfileTestData" sheetId="4" r:id="rId6"/>
+    <sheet name="SearchTestData" sheetId="5" r:id="rId7"/>
+    <sheet name="ChatTestData" sheetId="6" r:id="rId8"/>
+    <sheet name="ServiceDetailTestData" sheetId="7" r:id="rId9"/>
+    <sheet name="NotificationTestData" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
   <si>
     <t>Password</t>
   </si>
@@ -366,6 +367,15 @@
   </si>
   <si>
     <t>CompleteSentRequest</t>
+  </si>
+  <si>
+    <t>test.tester@gmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Pwd</t>
   </si>
 </sst>
 </file>
@@ -745,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8977337-D921-AC46-8E72-5A50572B2175}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,13 +766,11 @@
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -779,22 +787,10 @@
         <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -810,20 +806,8 @@
       <c r="E2">
         <v>123123</v>
       </c>
-      <c r="F2">
-        <v>123123</v>
-      </c>
-      <c r="G2">
-        <v>123456</v>
-      </c>
-      <c r="H2">
-        <v>123456</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="F2" t="s">
         <v>52</v>
-      </c>
-      <c r="J2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +819,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DB0938-B6C7-D347-8077-95E3356780A2}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDD637B-99C7-7B42-BAE6-F88E174063E1}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2">
+        <v>123123</v>
+      </c>
+      <c r="C2">
+        <v>123123</v>
+      </c>
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{79E77408-E72F-0B43-82BC-84590347AD6B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DEC66E-F359-7849-9BD4-2D798B9625ED}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -938,7 +1016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290D7D83-3F7A-424F-9F63-957F1296DE9C}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -1050,11 +1128,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E98292-C7AA-0B49-8379-1D04C9675C65}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1100,7 +1178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3722FA-74CF-BD4E-9CCF-CBC7308E1A3D}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -1242,7 +1320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABAFBA3-8E38-1348-967F-3A970261E0D5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1270,7 +1348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1FE9BE-FF0B-804A-BEFE-01AF06A9AB3F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1298,7 +1376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B58F33-06EC-A44B-8F98-DBAA495BC28A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1331,32 +1409,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DB0938-B6C7-D347-8077-95E3356780A2}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>